<commit_message>
Project and Sprint Backlog updated
- inserted specific dates (work days) in sprint backlog
- made new product backlog for this iteration
</commit_message>
<xml_diff>
--- a/Project Documentation/SPRINT_2.xlsx
+++ b/Project Documentation/SPRINT_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikol\Desktop\N\FiremanPro\Project Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Backlog Item</t>
   </si>
@@ -40,18 +40,6 @@
     <t>Original Estimate</t>
   </si>
   <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -67,36 +55,6 @@
     <t>Working days during sprint</t>
   </si>
   <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>Day 10</t>
-  </si>
-  <si>
-    <t>Day 11</t>
-  </si>
-  <si>
-    <t>Day 12</t>
-  </si>
-  <si>
-    <t>Day 13</t>
-  </si>
-  <si>
-    <t>Day 14</t>
-  </si>
-  <si>
-    <t>Day 15</t>
-  </si>
-  <si>
     <t>Team Member</t>
   </si>
   <si>
@@ -133,22 +91,6 @@
     <t>Popravci iz prošlog sprinta</t>
   </si>
   <si>
-    <r>
-      <t>Day 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(2.11.)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">usavršavanje baze podataka </t>
   </si>
   <si>
@@ -221,15 +163,9 @@
     <t>Effort (real)</t>
   </si>
   <si>
-    <t>isto</t>
-  </si>
-  <si>
     <t>SAD</t>
   </si>
   <si>
-    <t>gotov</t>
-  </si>
-  <si>
     <t>80(?)</t>
   </si>
   <si>
@@ -239,17 +175,77 @@
     <t>prikazivanje lokacije kuće na google karti</t>
   </si>
   <si>
-    <t>Sprint Backlog - 2. sprint (2.11. - 30.11)</t>
-  </si>
-  <si>
     <t>14 dana</t>
+  </si>
+  <si>
+    <t>2.11.</t>
+  </si>
+  <si>
+    <t>8.11.</t>
+  </si>
+  <si>
+    <t>7.11.</t>
+  </si>
+  <si>
+    <t>14.11.</t>
+  </si>
+  <si>
+    <t>15.11.</t>
+  </si>
+  <si>
+    <t>17.11.</t>
+  </si>
+  <si>
+    <t>18.11.</t>
+  </si>
+  <si>
+    <t>21.11.</t>
+  </si>
+  <si>
+    <t>22.11.</t>
+  </si>
+  <si>
+    <t>25.11.</t>
+  </si>
+  <si>
+    <t>27.11.</t>
+  </si>
+  <si>
+    <t>28.11.</t>
+  </si>
+  <si>
+    <t>29.11.</t>
+  </si>
+  <si>
+    <t>30.11.</t>
+  </si>
+  <si>
+    <t>Sprint Backlog - 2. sprint (2.11. - 30.11.)</t>
+  </si>
+  <si>
+    <t>Pretraživanje kuća</t>
+  </si>
+  <si>
+    <t>Prikaz plana kuće (tlocrt)</t>
+  </si>
+  <si>
+    <t>Prikaz lokacije najbližih hidranata</t>
+  </si>
+  <si>
+    <t>Kreiranje zapisnika intervencije</t>
+  </si>
+  <si>
+    <t>Slanje zapisnika na mail</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +324,22 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -386,13 +398,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,7 +490,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -508,16 +520,25 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,40 +552,46 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Isticanje2" xfId="1" builtinId="34"/>
+    <cellStyle name="20% - Isticanje3" xfId="2" builtinId="38"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -587,7 +614,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="hr-HR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -625,6 +652,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,6 +743,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -734,63 +763,60 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$S$6</c:f>
+              <c:f>'Sprint Backlog'!$E$6:$R$6</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>Day 1(2.11.)</c:v>
+                  <c:v>2.11.</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 2</c:v>
+                  <c:v>7.11.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 3</c:v>
+                  <c:v>8.11.</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 4</c:v>
+                  <c:v>14.11.</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 5</c:v>
+                  <c:v>15.11.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 6</c:v>
+                  <c:v>17.11.</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 7</c:v>
+                  <c:v>18.11.</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 8</c:v>
+                  <c:v>21.11.</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 9</c:v>
+                  <c:v>22.11.</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Day 10</c:v>
+                  <c:v>25.11.</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Day 11</c:v>
+                  <c:v>27.11.</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Day 12</c:v>
+                  <c:v>28.11.</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Day 13</c:v>
+                  <c:v>29.11.</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Day 14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Day 15</c:v>
+                  <c:v>30.11.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$22:$S$22</c:f>
+              <c:f>'Sprint Backlog'!$D$22:$R$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>102</c:v>
                 </c:pt>
@@ -865,6 +891,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -971,6 +998,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1674,13 +1702,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -2032,31 +2060,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y126"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X126"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.5" customWidth="1"/>
-    <col min="2" max="2" width="26.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" customWidth="1"/>
-    <col min="5" max="5" width="10.296875" customWidth="1"/>
-    <col min="6" max="6" width="6.69921875" customWidth="1"/>
-    <col min="7" max="7" width="7.796875" customWidth="1"/>
-    <col min="8" max="19" width="6.69921875" customWidth="1"/>
+    <col min="2" max="2" width="26.25" customWidth="1"/>
+    <col min="3" max="3" width="12.25" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="6.75" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
+    <col min="8" max="18" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:24" ht="27" x14ac:dyDescent="0.5">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -2072,15 +2100,14 @@
       <c r="P1" s="13"/>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2105,9 +2132,8 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2131,11 +2157,10 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-    </row>
-    <row r="4" spans="1:25" ht="23.4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2160,9 +2185,8 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2187,9 +2211,8 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" spans="1:25" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:24" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2202,61 +2225,58 @@
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
+      <c r="E6" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="R6" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-    </row>
-    <row r="7" spans="1:25" ht="27.6" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:24" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2278,179 +2298,172 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="15"/>
+      <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-    </row>
-    <row r="8" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27">
+    </row>
+    <row r="8" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17">
         <v>2</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="30"/>
-    </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27">
+      <c r="E8" s="33"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+    </row>
+    <row r="9" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17">
         <v>15</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="30"/>
-    </row>
-    <row r="10" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27">
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+    </row>
+    <row r="10" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17">
         <v>2</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="30"/>
-    </row>
-    <row r="11" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27">
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+    </row>
+    <row r="11" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17">
         <v>5</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="30"/>
-    </row>
-    <row r="12" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27">
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+    </row>
+    <row r="12" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17">
         <v>5</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="30"/>
-    </row>
-    <row r="13" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27">
+      <c r="E12" s="18"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+    </row>
+    <row r="13" spans="1:24" s="4" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
         <v>3</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="30"/>
-    </row>
-    <row r="14" spans="1:25" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
-        <v>32</v>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+    </row>
+    <row r="14" spans="1:24" ht="26.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2472,20 +2485,19 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="15"/>
+      <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3">
@@ -2505,20 +2517,19 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
+      <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3">
@@ -2538,20 +2549,19 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3">
@@ -2571,17 +2581,16 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-    </row>
-    <row r="18" spans="1:25" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2603,20 +2612,19 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3">
@@ -2636,20 +2644,19 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3">
@@ -2669,20 +2676,19 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3">
@@ -2702,17 +2708,16 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-    </row>
-    <row r="22" spans="1:25" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:24" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2734,15 +2739,14 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
+      <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2767,9 +2771,8 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2794,286 +2797,288 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-    </row>
-    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-    </row>
-    <row r="27" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="M27" s="23"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
+    </row>
+    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="40"/>
+      <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-    </row>
-    <row r="28" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="16">
+    </row>
+    <row r="28" spans="1:24" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="27"/>
+      <c r="H28" s="29">
         <v>12</v>
       </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="24">
+      <c r="I28" s="30"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="23">
         <v>3</v>
       </c>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24">
-        <f>L28*H28</f>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23">
+        <f>K28*H28</f>
         <v>36</v>
       </c>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="41"/>
+      <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-    </row>
-    <row r="29" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="16">
+    </row>
+    <row r="29" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="29">
         <v>11</v>
       </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="16">
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="29">
         <v>3</v>
       </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="24">
-        <f t="shared" ref="O29:O32" si="0">L29*H29</f>
+      <c r="L29" s="30"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="23">
+        <f>K29*H29</f>
         <v>33</v>
       </c>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="41"/>
+      <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-    </row>
-    <row r="30" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="16">
+        <v>7</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="H30" s="29">
         <v>13</v>
       </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="29">
         <v>2</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="24">
-        <f t="shared" si="0"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="23">
+        <f>K30*H30</f>
         <v>26</v>
       </c>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="41"/>
+      <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-    </row>
-    <row r="31" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="27"/>
+      <c r="H31" s="29">
         <v>12</v>
       </c>
-      <c r="B31" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="22"/>
-      <c r="H31" s="16">
-        <v>12</v>
-      </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="16">
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="29">
         <v>4</v>
       </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="24">
-        <f t="shared" si="0"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="23">
+        <f>K31*H31</f>
         <v>48</v>
       </c>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="41"/>
+      <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
       <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-    </row>
-    <row r="32" spans="1:25" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="16">
+    </row>
+    <row r="32" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="27"/>
+      <c r="H32" s="29">
         <v>10</v>
       </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="16">
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="29">
         <v>3</v>
       </c>
-      <c r="M32" s="17"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="24">
-        <f t="shared" si="0"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="23">
+        <f>K32*H32</f>
         <v>30</v>
       </c>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="41"/>
+      <c r="S32" s="4"/>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
       <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="P33">
-        <f>SUM(O28:Q32)</f>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33">
+        <f>SUM(N28:P32)</f>
         <v>173</v>
       </c>
+      <c r="S33" s="4"/>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
       <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
       <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
       <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
       <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
-      <c r="Y38" s="4"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S39" s="4"/>
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
-      <c r="Y39" s="4"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S40" s="4"/>
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="S41" s="4"/>
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
       <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -3098,9 +3103,8 @@
       <c r="V42" s="4"/>
       <c r="W42" s="4"/>
       <c r="X42" s="4"/>
-      <c r="Y42" s="4"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3125,9 +3129,8 @@
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
       <c r="X43" s="4"/>
-      <c r="Y43" s="4"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -3152,9 +3155,8 @@
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
       <c r="X44" s="4"/>
-      <c r="Y44" s="4"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3179,9 +3181,8 @@
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
-      <c r="Y45" s="4"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -3206,9 +3207,8 @@
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
       <c r="X46" s="4"/>
-      <c r="Y46" s="4"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3233,9 +3233,8 @@
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
       <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -3260,9 +3259,8 @@
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
       <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3287,9 +3285,8 @@
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -3314,9 +3311,8 @@
       <c r="V50" s="4"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>
-      <c r="Y50" s="4"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3341,9 +3337,8 @@
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
       <c r="X51" s="4"/>
-      <c r="Y51" s="4"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3368,9 +3363,8 @@
       <c r="V52" s="4"/>
       <c r="W52" s="4"/>
       <c r="X52" s="4"/>
-      <c r="Y52" s="4"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -3395,9 +3389,8 @@
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
       <c r="X53" s="4"/>
-      <c r="Y53" s="4"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -3422,9 +3415,8 @@
       <c r="V54" s="4"/>
       <c r="W54" s="4"/>
       <c r="X54" s="4"/>
-      <c r="Y54" s="4"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -3449,9 +3441,8 @@
       <c r="V55" s="4"/>
       <c r="W55" s="4"/>
       <c r="X55" s="4"/>
-      <c r="Y55" s="4"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3476,9 +3467,8 @@
       <c r="V56" s="4"/>
       <c r="W56" s="4"/>
       <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -3503,9 +3493,8 @@
       <c r="V57" s="4"/>
       <c r="W57" s="4"/>
       <c r="X57" s="4"/>
-      <c r="Y57" s="4"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -3530,9 +3519,8 @@
       <c r="V58" s="4"/>
       <c r="W58" s="4"/>
       <c r="X58" s="4"/>
-      <c r="Y58" s="4"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3557,9 +3545,8 @@
       <c r="V59" s="4"/>
       <c r="W59" s="4"/>
       <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3584,9 +3571,8 @@
       <c r="V60" s="4"/>
       <c r="W60" s="4"/>
       <c r="X60" s="4"/>
-      <c r="Y60" s="4"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -3611,9 +3597,8 @@
       <c r="V61" s="4"/>
       <c r="W61" s="4"/>
       <c r="X61" s="4"/>
-      <c r="Y61" s="4"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -3638,9 +3623,8 @@
       <c r="V62" s="4"/>
       <c r="W62" s="4"/>
       <c r="X62" s="4"/>
-      <c r="Y62" s="4"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -3665,9 +3649,8 @@
       <c r="V63" s="4"/>
       <c r="W63" s="4"/>
       <c r="X63" s="4"/>
-      <c r="Y63" s="4"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3692,9 +3675,8 @@
       <c r="V64" s="4"/>
       <c r="W64" s="4"/>
       <c r="X64" s="4"/>
-      <c r="Y64" s="4"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -3719,9 +3701,8 @@
       <c r="V65" s="4"/>
       <c r="W65" s="4"/>
       <c r="X65" s="4"/>
-      <c r="Y65" s="4"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -3746,9 +3727,8 @@
       <c r="V66" s="4"/>
       <c r="W66" s="4"/>
       <c r="X66" s="4"/>
-      <c r="Y66" s="4"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3773,9 +3753,8 @@
       <c r="V67" s="4"/>
       <c r="W67" s="4"/>
       <c r="X67" s="4"/>
-      <c r="Y67" s="4"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3800,9 +3779,8 @@
       <c r="V68" s="4"/>
       <c r="W68" s="4"/>
       <c r="X68" s="4"/>
-      <c r="Y68" s="4"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -3827,9 +3805,8 @@
       <c r="V69" s="4"/>
       <c r="W69" s="4"/>
       <c r="X69" s="4"/>
-      <c r="Y69" s="4"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -3854,9 +3831,8 @@
       <c r="V70" s="4"/>
       <c r="W70" s="4"/>
       <c r="X70" s="4"/>
-      <c r="Y70" s="4"/>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -3881,9 +3857,8 @@
       <c r="V71" s="4"/>
       <c r="W71" s="4"/>
       <c r="X71" s="4"/>
-      <c r="Y71" s="4"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -3908,9 +3883,8 @@
       <c r="V72" s="4"/>
       <c r="W72" s="4"/>
       <c r="X72" s="4"/>
-      <c r="Y72" s="4"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -3935,9 +3909,8 @@
       <c r="V73" s="4"/>
       <c r="W73" s="4"/>
       <c r="X73" s="4"/>
-      <c r="Y73" s="4"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -3962,9 +3935,8 @@
       <c r="V74" s="4"/>
       <c r="W74" s="4"/>
       <c r="X74" s="4"/>
-      <c r="Y74" s="4"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -3989,9 +3961,8 @@
       <c r="V75" s="4"/>
       <c r="W75" s="4"/>
       <c r="X75" s="4"/>
-      <c r="Y75" s="4"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4016,9 +3987,8 @@
       <c r="V76" s="4"/>
       <c r="W76" s="4"/>
       <c r="X76" s="4"/>
-      <c r="Y76" s="4"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -4043,9 +4013,8 @@
       <c r="V77" s="4"/>
       <c r="W77" s="4"/>
       <c r="X77" s="4"/>
-      <c r="Y77" s="4"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -4070,9 +4039,8 @@
       <c r="V78" s="4"/>
       <c r="W78" s="4"/>
       <c r="X78" s="4"/>
-      <c r="Y78" s="4"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -4097,9 +4065,8 @@
       <c r="V79" s="4"/>
       <c r="W79" s="4"/>
       <c r="X79" s="4"/>
-      <c r="Y79" s="4"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -4124,9 +4091,8 @@
       <c r="V80" s="4"/>
       <c r="W80" s="4"/>
       <c r="X80" s="4"/>
-      <c r="Y80" s="4"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -4151,9 +4117,8 @@
       <c r="V81" s="4"/>
       <c r="W81" s="4"/>
       <c r="X81" s="4"/>
-      <c r="Y81" s="4"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -4178,9 +4143,8 @@
       <c r="V82" s="4"/>
       <c r="W82" s="4"/>
       <c r="X82" s="4"/>
-      <c r="Y82" s="4"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -4205,9 +4169,8 @@
       <c r="V83" s="4"/>
       <c r="W83" s="4"/>
       <c r="X83" s="4"/>
-      <c r="Y83" s="4"/>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -4232,9 +4195,8 @@
       <c r="V84" s="4"/>
       <c r="W84" s="4"/>
       <c r="X84" s="4"/>
-      <c r="Y84" s="4"/>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -4259,9 +4221,8 @@
       <c r="V85" s="4"/>
       <c r="W85" s="4"/>
       <c r="X85" s="4"/>
-      <c r="Y85" s="4"/>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -4286,9 +4247,8 @@
       <c r="V86" s="4"/>
       <c r="W86" s="4"/>
       <c r="X86" s="4"/>
-      <c r="Y86" s="4"/>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -4313,9 +4273,8 @@
       <c r="V87" s="4"/>
       <c r="W87" s="4"/>
       <c r="X87" s="4"/>
-      <c r="Y87" s="4"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -4340,9 +4299,8 @@
       <c r="V88" s="4"/>
       <c r="W88" s="4"/>
       <c r="X88" s="4"/>
-      <c r="Y88" s="4"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -4367,9 +4325,8 @@
       <c r="V89" s="4"/>
       <c r="W89" s="4"/>
       <c r="X89" s="4"/>
-      <c r="Y89" s="4"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -4394,9 +4351,8 @@
       <c r="V90" s="4"/>
       <c r="W90" s="4"/>
       <c r="X90" s="4"/>
-      <c r="Y90" s="4"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -4421,9 +4377,8 @@
       <c r="V91" s="4"/>
       <c r="W91" s="4"/>
       <c r="X91" s="4"/>
-      <c r="Y91" s="4"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -4448,9 +4403,8 @@
       <c r="V92" s="4"/>
       <c r="W92" s="4"/>
       <c r="X92" s="4"/>
-      <c r="Y92" s="4"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -4475,9 +4429,8 @@
       <c r="V93" s="4"/>
       <c r="W93" s="4"/>
       <c r="X93" s="4"/>
-      <c r="Y93" s="4"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -4502,9 +4455,8 @@
       <c r="V94" s="4"/>
       <c r="W94" s="4"/>
       <c r="X94" s="4"/>
-      <c r="Y94" s="4"/>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -4529,9 +4481,8 @@
       <c r="V95" s="4"/>
       <c r="W95" s="4"/>
       <c r="X95" s="4"/>
-      <c r="Y95" s="4"/>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -4556,9 +4507,8 @@
       <c r="V96" s="4"/>
       <c r="W96" s="4"/>
       <c r="X96" s="4"/>
-      <c r="Y96" s="4"/>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -4583,9 +4533,8 @@
       <c r="V97" s="4"/>
       <c r="W97" s="4"/>
       <c r="X97" s="4"/>
-      <c r="Y97" s="4"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -4610,9 +4559,8 @@
       <c r="V98" s="4"/>
       <c r="W98" s="4"/>
       <c r="X98" s="4"/>
-      <c r="Y98" s="4"/>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -4637,9 +4585,8 @@
       <c r="V99" s="4"/>
       <c r="W99" s="4"/>
       <c r="X99" s="4"/>
-      <c r="Y99" s="4"/>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -4664,9 +4611,8 @@
       <c r="V100" s="4"/>
       <c r="W100" s="4"/>
       <c r="X100" s="4"/>
-      <c r="Y100" s="4"/>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -4691,9 +4637,8 @@
       <c r="V101" s="4"/>
       <c r="W101" s="4"/>
       <c r="X101" s="4"/>
-      <c r="Y101" s="4"/>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -4718,9 +4663,8 @@
       <c r="V102" s="4"/>
       <c r="W102" s="4"/>
       <c r="X102" s="4"/>
-      <c r="Y102" s="4"/>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -4745,9 +4689,8 @@
       <c r="V103" s="4"/>
       <c r="W103" s="4"/>
       <c r="X103" s="4"/>
-      <c r="Y103" s="4"/>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -4772,9 +4715,8 @@
       <c r="V104" s="4"/>
       <c r="W104" s="4"/>
       <c r="X104" s="4"/>
-      <c r="Y104" s="4"/>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -4799,9 +4741,8 @@
       <c r="V105" s="4"/>
       <c r="W105" s="4"/>
       <c r="X105" s="4"/>
-      <c r="Y105" s="4"/>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -4826,9 +4767,8 @@
       <c r="V106" s="4"/>
       <c r="W106" s="4"/>
       <c r="X106" s="4"/>
-      <c r="Y106" s="4"/>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -4853,9 +4793,8 @@
       <c r="V107" s="4"/>
       <c r="W107" s="4"/>
       <c r="X107" s="4"/>
-      <c r="Y107" s="4"/>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -4880,9 +4819,8 @@
       <c r="V108" s="4"/>
       <c r="W108" s="4"/>
       <c r="X108" s="4"/>
-      <c r="Y108" s="4"/>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -4907,9 +4845,8 @@
       <c r="V109" s="4"/>
       <c r="W109" s="4"/>
       <c r="X109" s="4"/>
-      <c r="Y109" s="4"/>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -4934,9 +4871,8 @@
       <c r="V110" s="4"/>
       <c r="W110" s="4"/>
       <c r="X110" s="4"/>
-      <c r="Y110" s="4"/>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -4961,9 +4897,8 @@
       <c r="V111" s="4"/>
       <c r="W111" s="4"/>
       <c r="X111" s="4"/>
-      <c r="Y111" s="4"/>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -4988,9 +4923,8 @@
       <c r="V112" s="4"/>
       <c r="W112" s="4"/>
       <c r="X112" s="4"/>
-      <c r="Y112" s="4"/>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -5015,9 +4949,8 @@
       <c r="V113" s="4"/>
       <c r="W113" s="4"/>
       <c r="X113" s="4"/>
-      <c r="Y113" s="4"/>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -5042,9 +4975,8 @@
       <c r="V114" s="4"/>
       <c r="W114" s="4"/>
       <c r="X114" s="4"/>
-      <c r="Y114" s="4"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -5069,9 +5001,8 @@
       <c r="V115" s="4"/>
       <c r="W115" s="4"/>
       <c r="X115" s="4"/>
-      <c r="Y115" s="4"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -5096,9 +5027,8 @@
       <c r="V116" s="4"/>
       <c r="W116" s="4"/>
       <c r="X116" s="4"/>
-      <c r="Y116" s="4"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -5123,9 +5053,8 @@
       <c r="V117" s="4"/>
       <c r="W117" s="4"/>
       <c r="X117" s="4"/>
-      <c r="Y117" s="4"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -5150,9 +5079,8 @@
       <c r="V118" s="4"/>
       <c r="W118" s="4"/>
       <c r="X118" s="4"/>
-      <c r="Y118" s="4"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -5177,9 +5105,8 @@
       <c r="V119" s="4"/>
       <c r="W119" s="4"/>
       <c r="X119" s="4"/>
-      <c r="Y119" s="4"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -5204,9 +5131,8 @@
       <c r="V120" s="4"/>
       <c r="W120" s="4"/>
       <c r="X120" s="4"/>
-      <c r="Y120" s="4"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -5231,9 +5157,8 @@
       <c r="V121" s="4"/>
       <c r="W121" s="4"/>
       <c r="X121" s="4"/>
-      <c r="Y121" s="4"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -5258,9 +5183,8 @@
       <c r="V122" s="4"/>
       <c r="W122" s="4"/>
       <c r="X122" s="4"/>
-      <c r="Y122" s="4"/>
-    </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -5285,9 +5209,8 @@
       <c r="V123" s="4"/>
       <c r="W123" s="4"/>
       <c r="X123" s="4"/>
-      <c r="Y123" s="4"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5312,9 +5235,8 @@
       <c r="V124" s="4"/>
       <c r="W124" s="4"/>
       <c r="X124" s="4"/>
-      <c r="Y124" s="4"/>
-    </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -5339,9 +5261,8 @@
       <c r="V125" s="4"/>
       <c r="W125" s="4"/>
       <c r="X125" s="4"/>
-      <c r="Y125" s="4"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -5366,34 +5287,33 @@
       <c r="V126" s="4"/>
       <c r="W126" s="4"/>
       <c r="X126" s="4"/>
-      <c r="Y126" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="O31:Q31"/>
-    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="N32:P32"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="O28:Q28"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:P28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5407,145 +5327,691 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B9B8C9-1968-4B13-9363-CA720ABDACA7}">
-  <dimension ref="A3:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:DK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="36.69921875" customWidth="1"/>
-    <col min="4" max="4" width="6.296875" customWidth="1"/>
-    <col min="7" max="7" width="14.69921875" customWidth="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1"/>
+    <col min="4" max="4" width="6.25" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="34">
+    <row r="3" spans="1:115" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
+      <c r="CJ3"/>
+      <c r="CK3"/>
+      <c r="CL3"/>
+      <c r="CM3"/>
+      <c r="CN3"/>
+      <c r="CO3"/>
+      <c r="CP3"/>
+      <c r="CQ3"/>
+      <c r="CR3"/>
+      <c r="CS3"/>
+      <c r="CT3"/>
+      <c r="CU3"/>
+      <c r="CV3"/>
+      <c r="CW3"/>
+      <c r="CX3"/>
+      <c r="CY3"/>
+      <c r="CZ3"/>
+      <c r="DA3"/>
+      <c r="DB3"/>
+      <c r="DC3"/>
+      <c r="DD3"/>
+      <c r="DE3"/>
+      <c r="DF3"/>
+      <c r="DG3"/>
+      <c r="DH3"/>
+      <c r="DI3"/>
+      <c r="DJ3"/>
+      <c r="DK3"/>
+    </row>
+    <row r="4" spans="1:115" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="C4" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="36">
         <v>1</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="36">
         <v>1</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="36">
         <v>80</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="34">
+      <c r="G4" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+      <c r="AQ4"/>
+      <c r="AR4"/>
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+      <c r="BD4"/>
+      <c r="BE4"/>
+      <c r="BF4"/>
+      <c r="BG4"/>
+      <c r="BH4"/>
+      <c r="BI4"/>
+      <c r="BJ4"/>
+      <c r="BK4"/>
+      <c r="BL4"/>
+      <c r="BM4"/>
+      <c r="BN4"/>
+      <c r="BO4"/>
+      <c r="BP4"/>
+      <c r="BQ4"/>
+      <c r="BR4"/>
+      <c r="BS4"/>
+      <c r="BT4"/>
+      <c r="BU4"/>
+      <c r="BV4"/>
+      <c r="BW4"/>
+      <c r="BX4"/>
+      <c r="BY4"/>
+      <c r="BZ4"/>
+      <c r="CA4"/>
+      <c r="CB4"/>
+      <c r="CC4"/>
+      <c r="CD4"/>
+      <c r="CE4"/>
+      <c r="CF4"/>
+      <c r="CG4"/>
+      <c r="CH4"/>
+      <c r="CI4"/>
+      <c r="CJ4"/>
+      <c r="CK4"/>
+      <c r="CL4"/>
+      <c r="CM4"/>
+      <c r="CN4"/>
+      <c r="CO4"/>
+      <c r="CP4"/>
+      <c r="CQ4"/>
+      <c r="CR4"/>
+      <c r="CS4"/>
+      <c r="CT4"/>
+      <c r="CU4"/>
+      <c r="CV4"/>
+      <c r="CW4"/>
+      <c r="CX4"/>
+      <c r="CY4"/>
+      <c r="CZ4"/>
+      <c r="DA4"/>
+      <c r="DB4"/>
+      <c r="DC4"/>
+      <c r="DD4"/>
+      <c r="DE4"/>
+      <c r="DF4"/>
+      <c r="DG4"/>
+      <c r="DH4"/>
+      <c r="DI4"/>
+      <c r="DJ4"/>
+      <c r="DK4"/>
+    </row>
+    <row r="5" spans="1:115" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="C5" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="36">
         <v>2</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="36">
         <v>1</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="36">
         <v>35</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="36">
+      <c r="G5" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+      <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
+      <c r="BG5"/>
+      <c r="BH5"/>
+      <c r="BI5"/>
+      <c r="BJ5"/>
+      <c r="BK5"/>
+      <c r="BL5"/>
+      <c r="BM5"/>
+      <c r="BN5"/>
+      <c r="BO5"/>
+      <c r="BP5"/>
+      <c r="BQ5"/>
+      <c r="BR5"/>
+      <c r="BS5"/>
+      <c r="BT5"/>
+      <c r="BU5"/>
+      <c r="BV5"/>
+      <c r="BW5"/>
+      <c r="BX5"/>
+      <c r="BY5"/>
+      <c r="BZ5"/>
+      <c r="CA5"/>
+      <c r="CB5"/>
+      <c r="CC5"/>
+      <c r="CD5"/>
+      <c r="CE5"/>
+      <c r="CF5"/>
+      <c r="CG5"/>
+      <c r="CH5"/>
+      <c r="CI5"/>
+      <c r="CJ5"/>
+      <c r="CK5"/>
+      <c r="CL5"/>
+      <c r="CM5"/>
+      <c r="CN5"/>
+      <c r="CO5"/>
+      <c r="CP5"/>
+      <c r="CQ5"/>
+      <c r="CR5"/>
+      <c r="CS5"/>
+      <c r="CT5"/>
+      <c r="CU5"/>
+      <c r="CV5"/>
+      <c r="CW5"/>
+      <c r="CX5"/>
+      <c r="CY5"/>
+      <c r="CZ5"/>
+      <c r="DA5"/>
+      <c r="DB5"/>
+      <c r="DC5"/>
+      <c r="DD5"/>
+      <c r="DE5"/>
+      <c r="DF5"/>
+      <c r="DG5"/>
+      <c r="DH5"/>
+      <c r="DI5"/>
+      <c r="DJ5"/>
+      <c r="DK5"/>
+    </row>
+    <row r="6" spans="1:115" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="22">
         <v>3</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="36">
+      <c r="E6" s="22">
         <v>2</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="22">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="36">
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+      <c r="BD6"/>
+      <c r="BE6"/>
+      <c r="BF6"/>
+      <c r="BG6"/>
+      <c r="BH6"/>
+      <c r="BI6"/>
+      <c r="BJ6"/>
+      <c r="BK6"/>
+      <c r="BL6"/>
+      <c r="BM6"/>
+      <c r="BN6"/>
+      <c r="BO6"/>
+      <c r="BP6"/>
+      <c r="BQ6"/>
+      <c r="BR6"/>
+      <c r="BS6"/>
+      <c r="BT6"/>
+      <c r="BU6"/>
+      <c r="BV6"/>
+      <c r="BW6"/>
+      <c r="BX6"/>
+      <c r="BY6"/>
+      <c r="BZ6"/>
+      <c r="CA6"/>
+      <c r="CB6"/>
+      <c r="CC6"/>
+      <c r="CD6"/>
+      <c r="CE6"/>
+      <c r="CF6"/>
+      <c r="CG6"/>
+      <c r="CH6"/>
+      <c r="CI6"/>
+      <c r="CJ6"/>
+      <c r="CK6"/>
+      <c r="CL6"/>
+      <c r="CM6"/>
+      <c r="CN6"/>
+      <c r="CO6"/>
+      <c r="CP6"/>
+      <c r="CQ6"/>
+      <c r="CR6"/>
+      <c r="CS6"/>
+      <c r="CT6"/>
+      <c r="CU6"/>
+      <c r="CV6"/>
+      <c r="CW6"/>
+      <c r="CX6"/>
+      <c r="CY6"/>
+      <c r="CZ6"/>
+      <c r="DA6"/>
+      <c r="DB6"/>
+      <c r="DC6"/>
+      <c r="DD6"/>
+      <c r="DE6"/>
+      <c r="DF6"/>
+      <c r="DG6"/>
+      <c r="DH6"/>
+      <c r="DI6"/>
+      <c r="DJ6"/>
+      <c r="DK6"/>
+    </row>
+    <row r="7" spans="1:115" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="22">
         <v>4</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="36">
+      <c r="E7" s="22">
         <v>2</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="22">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8">
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7"/>
+      <c r="AY7"/>
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7"/>
+      <c r="BC7"/>
+      <c r="BD7"/>
+      <c r="BE7"/>
+      <c r="BF7"/>
+      <c r="BG7"/>
+      <c r="BH7"/>
+      <c r="BI7"/>
+      <c r="BJ7"/>
+      <c r="BK7"/>
+      <c r="BL7"/>
+      <c r="BM7"/>
+      <c r="BN7"/>
+      <c r="BO7"/>
+      <c r="BP7"/>
+      <c r="BQ7"/>
+      <c r="BR7"/>
+      <c r="BS7"/>
+      <c r="BT7"/>
+      <c r="BU7"/>
+      <c r="BV7"/>
+      <c r="BW7"/>
+      <c r="BX7"/>
+      <c r="BY7"/>
+      <c r="BZ7"/>
+      <c r="CA7"/>
+      <c r="CB7"/>
+      <c r="CC7"/>
+      <c r="CD7"/>
+      <c r="CE7"/>
+      <c r="CF7"/>
+      <c r="CG7"/>
+      <c r="CH7"/>
+      <c r="CI7"/>
+      <c r="CJ7"/>
+      <c r="CK7"/>
+      <c r="CL7"/>
+      <c r="CM7"/>
+      <c r="CN7"/>
+      <c r="CO7"/>
+      <c r="CP7"/>
+      <c r="CQ7"/>
+      <c r="CR7"/>
+      <c r="CS7"/>
+      <c r="CT7"/>
+      <c r="CU7"/>
+      <c r="CV7"/>
+      <c r="CW7"/>
+      <c r="CX7"/>
+      <c r="CY7"/>
+      <c r="CZ7"/>
+      <c r="DA7"/>
+      <c r="DB7"/>
+      <c r="DC7"/>
+      <c r="DD7"/>
+      <c r="DE7"/>
+      <c r="DF7"/>
+      <c r="DG7"/>
+      <c r="DH7"/>
+      <c r="DI7"/>
+      <c r="DJ7"/>
+      <c r="DK7"/>
+    </row>
+    <row r="8" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="B8" s="39"/>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
         <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="F8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9">
         <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10">
+      <c r="F9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
         <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>60</v>
+      <c r="F10">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>